<commit_message>
Adicionado a criacao de pasta ano e mes dentro da pasta PEDIDO
</commit_message>
<xml_diff>
--- a/TALAO/Exemplo Talao.xlsx
+++ b/TALAO/Exemplo Talao.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Estudo Python\Planilhas Mae\TALAO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Estudo Python\Planilhas Mae\AutomacaoRelatorioPedidos\TALAO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCA80AC-33AC-49D6-813B-C830F88D5D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E704CE27-C5CD-4ABF-8CBD-83666D593387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Página3" sheetId="1" r:id="rId1"/>
@@ -1052,7 +1052,9 @@
             <v>51</v>
           </cell>
           <cell r="B52"/>
-          <cell r="C52"/>
+          <cell r="C52" t="str">
+            <v>Rest Gil</v>
+          </cell>
           <cell r="D52"/>
           <cell r="E52"/>
           <cell r="F52"/>

</xml_diff>